<commit_message>
new mice, and deleting mice that did not get used
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_150316_B.xlsx
+++ b/Mouse_workbooks/CH_150316_B.xlsx
@@ -130,25 +130,25 @@
     <t>4% PFA</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>EMX+/-</t>
+  </si>
+  <si>
+    <t>Burr hole injection</t>
+  </si>
+  <si>
     <t>CH_150316_B</t>
   </si>
   <si>
-    <t>Male?</t>
-  </si>
-  <si>
-    <t>EMX+/-   C57</t>
-  </si>
-  <si>
-    <t>R ear tag</t>
-  </si>
-  <si>
-    <t>Injected with oChIEF(km) into V1. Testing to see if the construct from UPENN is functional</t>
-  </si>
-  <si>
-    <t>Burr hole injection</t>
-  </si>
-  <si>
-    <t>injected 300nl, at 2.56 left of lambda, 350 to 500 um from pia. Injected the rAAV2/1.DIO.EF1a.oChIEF(km).dTomato constuct from UPENN. A small amount of backflow.</t>
+    <t>Right ear tag</t>
+  </si>
+  <si>
+    <t>injected the UPENN version of the oCHIEF kinetic mutant. No real physiology, but good histology showing retrograde infection?</t>
+  </si>
+  <si>
+    <t>Injected 300 nl at 2.56 mm left of Lambda, -380 um from pia. This is the AAV1.EF1a.DIO.oCHIEF(ET/TC).dTomato from UPENN. Some backflow.</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="38" customHeight="1">
@@ -1305,7 +1305,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="38" customHeight="1">
@@ -1313,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="33">
-        <v>42060</v>
+        <v>42057</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="38" customHeight="1">
@@ -1321,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="38" customHeight="1">
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
@@ -1337,7 +1337,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="38" hidden="1" customHeight="1" thickTop="1"/>
@@ -2749,7 +2749,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G7"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
@@ -2789,7 +2789,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>

</xml_diff>